<commit_message>
ecs事件 增加beforeupdate 和 lateupdate
</commit_message>
<xml_diff>
--- a/Excel/Language/_Common.xlsx
+++ b/Excel/Language/_Common.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12435" activeTab="2"/>
+    <workbookView windowWidth="32265" windowHeight="15060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>字段</t>
   </si>
   <si>
-    <t>描述</t>
-  </si>
-  <si>
     <t>类型</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>xx</t>
   </si>
   <si>
     <t>草泥马</t>
@@ -1098,18 +1092,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" spans="1:5">
+    <row r="1" ht="12" customHeight="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1122,78 +1116,63 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="3:4">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="4:5">
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1206,15 +1185,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B$1:B$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" spans="1:5">
+    <row r="1" ht="12" customHeight="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1227,78 +1206,63 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="3:4">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="4:5">
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1311,15 +1275,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" ht="12" customHeight="1" spans="1:5">
+    <row r="1" ht="12" customHeight="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1332,78 +1296,63 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="3:4">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="4:5">
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>